<commit_message>
Atualização automática de ESTEIO.xlsx
</commit_message>
<xml_diff>
--- a/ESTEIO.xlsx
+++ b/ESTEIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEA16E0D-0582-41CA-B7C8-A5FBBB48CB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{013C219D-11CB-48B1-8DBF-88C1D3DCD5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,20 +21,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1083,7 +1070,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1143,36 +1130,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1211,14 +1174,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1263,7 +1221,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{F549B427-901C-430E-B4A8-CE750BB38068}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{31BE65AB-E5D9-4946-8225-D903A1524169}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1293,10 +1251,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1317BF4-5166-4BDF-BBEF-5033E47C7C61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26C7A094-23EA-43A2-A484-71984C197DC6}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1334,7 +1292,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191217E9-18BE-4E23-8B83-BB3D59C1ACFC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F2BC796-B1EC-4253-8004-C3A82F0BFE0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1397,7 +1355,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F350D8DD-E549-4986-8110-9ADB5726EF10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACFBC29E-C23E-4B31-96B4-19F2F44D2479}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1374,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A14AF877-57B3-1FE2-424D-92AC029AFDE4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0E34AF4-50B2-F981-9CD8-E96116315F7A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1465,7 +1423,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24A17635-3ED2-DC2B-3A61-25B1B4413A74}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E166EBE-7DBC-51A4-27D5-F7DE905EA4BF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1484,7 +1442,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16EB889-D980-F00A-7AED-4C4C0B2EEDC2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C224D030-0E11-893B-0903-5D56EB57E5D6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1515,7 +1473,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{002A084A-72CC-2407-F147-1B27B85A7B80}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A58D7E7-0015-FFF5-8D45-289BC0B50CF1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1546,7 +1504,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CB6FC34-6174-D5DE-790A-5DC1023A30ED}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EFBB9A4-A0C3-7694-16F6-6CDE4C1DC659}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1589,7 +1547,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A524AF9-BE43-498D-B2DA-C4106F9B9B77}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFCE9D3A-8A00-436D-B502-9E37CCBAA1D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1627,7 +1585,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F73ED95-929B-4711-B31C-9CC7D7469CAE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FAC6B70-A61E-4755-9CCC-667E15B21E3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1670,7 +1628,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A97684FD-69C2-47D5-AE77-E6B7EDDC7E90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB2437CA-1051-47EB-B3F0-FBEC9A60B8D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1983,7 +1941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF44974-79B7-43B1-B307-35FC9D7804E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C463F1A7-9DB3-4E08-BE3E-7FF2C3EC7CB9}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1995,98 +1953,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="36"/>
-    <col min="6" max="6" width="2" style="36" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="36" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="36"/>
+    <col min="1" max="5" width="12.5703125" style="33"/>
+    <col min="6" max="6" width="2" style="33" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="33" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="35"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="35"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="35"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="35"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="35"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="35"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="35"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="35"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="35"/>
+      <c r="F9" s="32"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="35"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="35"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="35"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="35"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="35"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="35"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="35"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="35"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="35"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="35"/>
+      <c r="F19" s="32"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="35"/>
+      <c r="F20" s="32"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="35"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="35"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="35"/>
+      <c r="F23" s="32"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="35"/>
+      <c r="F24" s="32"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="35"/>
+      <c r="F25" s="32"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="35"/>
+      <c r="F26" s="32"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="35"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="35"/>
+      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="35"/>
+      <c r="F29" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5350,19 +5308,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5385,101 +5343,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="19" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5504,54 +5462,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="20" t="s">
         <v>300</v>
       </c>
     </row>
@@ -5562,43 +5521,43 @@
       <c r="B2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="23">
         <v>45078</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="24">
         <v>4252</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="25">
         <v>37179</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="25">
         <v>3110</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="26" t="s">
         <v>303</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="26" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5629,25 +5588,24 @@
       <c r="B1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>306</v>
       </c>
-      <c r="E1" s="31">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="28">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="31">
         <v>129</v>
       </c>
-      <c r="F1" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>307</v>
-      </c>
-      <c r="B2" s="34">
-        <v>129</v>
-      </c>
-      <c r="C2" s="32">
+      <c r="C2" s="29">
         <v>8.5306176431688922E-3</v>
       </c>
     </row>

</xml_diff>